<commit_message>
fixed uniswap v2 scripts
</commit_message>
<xml_diff>
--- a/uniswap_v2_optimism.xlsx
+++ b/uniswap_v2_optimism.xlsx
@@ -4,10 +4,444 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="ethereum_uniswap_v2_2.xlsx" state="visible" r:id="rId3"/>
+    <sheet sheetId="1" name="optimism_uniswap_v2.xlsx" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="143">
+  <si>
+    <t>Sr no.</t>
+  </si>
+  <si>
+    <t>Pair address</t>
+  </si>
+  <si>
+    <t>Token 0</t>
+  </si>
+  <si>
+    <t>Token 0 ID</t>
+  </si>
+  <si>
+    <t>Token 1</t>
+  </si>
+  <si>
+    <t>Token 1 ID</t>
+  </si>
+  <si>
+    <t>Liquidity</t>
+  </si>
+  <si>
+    <t>0x4C43646304492A925E335f2b6d840C1489f17815</t>
+  </si>
+  <si>
+    <t>USD Coin (USDC)</t>
+  </si>
+  <si>
+    <t>0x0b2C639c533813f4Aa9D7837CAf62653d097Ff85</t>
+  </si>
+  <si>
+    <t>Wrapped Ether (WETH)</t>
+  </si>
+  <si>
+    <t>0x4200000000000000000000000000000000000006</t>
+  </si>
+  <si>
+    <t>304148429 USD Coin (USDC) + 87094439095421390 Wrapped Ether (WETH)</t>
+  </si>
+  <si>
+    <t>0x895bb8b1Cc9746b431B66B2114f46A7A57412980</t>
+  </si>
+  <si>
+    <t>Frax (FRAX)</t>
+  </si>
+  <si>
+    <t>0x2E3D870790dC77A83DD1d18184Acc7439A53f475</t>
+  </si>
+  <si>
+    <t>20028257108434192180 Frax (FRAX) + 5663984903474051 Wrapped Ether (WETH)</t>
+  </si>
+  <si>
+    <t>0x8782Edc55C8514BF30e36A3585AfCadbFF525C77</t>
+  </si>
+  <si>
+    <t>Wrapped BTC (WBTC)</t>
+  </si>
+  <si>
+    <t>0x68f180fcCe6836688e9084f035309E29Bf0A2095</t>
+  </si>
+  <si>
+    <t>351632762136396175 Wrapped Ether (WETH) + 1846221 Wrapped BTC (WBTC)</t>
+  </si>
+  <si>
+    <t>0xf3fe89650E170D4d54D8dDd41AfFDE7369cBc7d3</t>
+  </si>
+  <si>
+    <t>Optimism (OP)</t>
+  </si>
+  <si>
+    <t>0x4200000000000000000000000000000000000042</t>
+  </si>
+  <si>
+    <t>2220706402880144 Wrapped Ether (WETH) + 2367040885388348825 Optimism (OP)</t>
+  </si>
+  <si>
+    <t>0x472CeDE4a60CB6Bbc310664d6a23E58c23F877b9</t>
+  </si>
+  <si>
+    <t>DINERO (DINERO)</t>
+  </si>
+  <si>
+    <t>0xBe827F2975f2da78feb3683c558B143E3C6dCD07</t>
+  </si>
+  <si>
+    <t>24760 Wrapped BTC (WBTC) + 226531014 DINERO (DINERO)</t>
+  </si>
+  <si>
+    <t>0xFfee909C673b41E6F532CD1fF5D531fBAEE6CdcE</t>
+  </si>
+  <si>
+    <t>LSD DAO (LSD)</t>
+  </si>
+  <si>
+    <t>0xAb1047894dA4ec207c71bE0AEF5c7885e07B2DaF</t>
+  </si>
+  <si>
+    <t>361830603626364 Wrapped Ether (WETH) + 16181533412262228063737423 LSD DAO (LSD)</t>
+  </si>
+  <si>
+    <t>0xA7A8bFa77133a5A984c18e1CA898541D3C86A3D5</t>
+  </si>
+  <si>
+    <t>Shih Tzu (SHIH)</t>
+  </si>
+  <si>
+    <t>0x9Fe7aC2F13B968c607fc0F2ad7EFB1FD1eDD9c36</t>
+  </si>
+  <si>
+    <t>6 Optimism (OP) + 195376 Shih Tzu (SHIH)</t>
+  </si>
+  <si>
+    <t>0x2f629782C58918252970Ab038D3FBD16E84D5076</t>
+  </si>
+  <si>
+    <t>Tether USD (USDT)</t>
+  </si>
+  <si>
+    <t>0x94b008aA00579c1307B0EF2c499aD98a8ce58e58</t>
+  </si>
+  <si>
+    <t>555103037446626 Wrapped Ether (WETH) + 1936004 Tether USD (USDT)</t>
+  </si>
+  <si>
+    <t>0x6728bfC6F086801C6fdAA8a3689fF498Ed071704</t>
+  </si>
+  <si>
+    <t>1000 USD Coin (USDC) + 1001 Tether USD (USDT)</t>
+  </si>
+  <si>
+    <t>0x57402AB043e02f0C54103214AA8a4B1Ae941eb9b</t>
+  </si>
+  <si>
+    <t>ChainLink Token (LINK)</t>
+  </si>
+  <si>
+    <t>0x350a791Bfc2C21F9Ed5d10980Dad2e2638ffa7f6</t>
+  </si>
+  <si>
+    <t>0x7F5c764cBc14f9669B88837ca1490cCa17c31607</t>
+  </si>
+  <si>
+    <t>60744464486785 ChainLink Token (LINK) + 100 USD Coin (USDC)</t>
+  </si>
+  <si>
+    <t>0x20aA6817f2CF9F3fAa91D3F7Bba6B4f323A42A46</t>
+  </si>
+  <si>
+    <t>Tether (USDT)</t>
+  </si>
+  <si>
+    <t>0x0C85dA204b9E46e79AA8cfE4725c4b11ea0dE20d</t>
+  </si>
+  <si>
+    <t>10085080250 Tether (USDT) + 9915988898969884 Wrapped Ether (WETH)</t>
+  </si>
+  <si>
+    <t>0xBa70b451ff20b05F6815B2a0F439900c6fAc1E89</t>
+  </si>
+  <si>
+    <t>TOKS (TOKS)</t>
+  </si>
+  <si>
+    <t>0x95e5E616C008D37b1956508c36d7258c3B30Ad56</t>
+  </si>
+  <si>
+    <t>9950397506050098 Wrapped Ether (WETH) + 1005000000000000000000 TOKS (TOKS)</t>
+  </si>
+  <si>
+    <t>0xCf00aFB9cC16253D4856A4d3EE9435e195022406</t>
+  </si>
+  <si>
+    <t>TokenWithFee (TokenWithFee)</t>
+  </si>
+  <si>
+    <t>0x487b38a4FB835DAED214932aF407b8321E25C799</t>
+  </si>
+  <si>
+    <t>1017006846095545 Wrapped Ether (WETH) + 973493612131591400606 TokenWithFee (TokenWithFee)</t>
+  </si>
+  <si>
+    <t>0x41F0EC06d0106f79cb01abf7bE1D086721ff91dd</t>
+  </si>
+  <si>
+    <t>Synthetix Network Token (SNX)</t>
+  </si>
+  <si>
+    <t>0x8700dAec35aF8Ff88c16BdF0418774CB3D7599B4</t>
+  </si>
+  <si>
+    <t>7561689 USD Coin (USDC) + 1863914599492459355 Synthetix Network Token (SNX)</t>
+  </si>
+  <si>
+    <t>0x1b9B44632688bB2Af6F816a61960c34fa56ace2b</t>
+  </si>
+  <si>
+    <t>Worldcoin (WLD)</t>
+  </si>
+  <si>
+    <t>0xdC6fF44d5d932Cbd77B52E5612Ba0529DC6226F1</t>
+  </si>
+  <si>
+    <t>56711835801793594 Wrapped Ether (WETH) + 22617296403473244729 Worldcoin (WLD)</t>
+  </si>
+  <si>
+    <t>0x7b223a503964c0f5F12b9C3f9d977b21a83Da24f</t>
+  </si>
+  <si>
+    <t>203470696640210319 Optimism (OP) + 688384 USD Coin (USDC)</t>
+  </si>
+  <si>
+    <t>0xF068e94E72281ea2D0AEab4dCD40F8B21B3830Aa</t>
+  </si>
+  <si>
+    <t>Wrapped liquid staked Ether 2.0 (wstETH)</t>
+  </si>
+  <si>
+    <t>0x1F32b1c2345538c0c6f582fCB022739c4A194Ebb</t>
+  </si>
+  <si>
+    <t>1000000000000000 Wrapped liquid staked Ether 2.0 (wstETH) + 55000000 DINERO (DINERO)</t>
+  </si>
+  <si>
+    <t>0x1EbDf8Cc73DB0f42383a0aA1ca872076b019abd7</t>
+  </si>
+  <si>
+    <t>Aave Token (AAVE)</t>
+  </si>
+  <si>
+    <t>0x76FB31fb4af56892A25e32cFC43De717950c9278</t>
+  </si>
+  <si>
+    <t>186 Wrapped Ether (WETH) + 5410 Aave Token (AAVE)</t>
+  </si>
+  <si>
+    <t>0x4117Bd14EED31383034B186f2823cbC53bC14382</t>
+  </si>
+  <si>
+    <t>tst (tst)</t>
+  </si>
+  <si>
+    <t>0x6C51303Bf4e51FD44F6bB07aE2c7267f15E35910</t>
+  </si>
+  <si>
+    <t>1 Wrapped Ether (WETH) + 10000000 tst (tst)</t>
+  </si>
+  <si>
+    <t>0x3EeE6F7173FaF13e25669C1A0EaDbfdB41d3BE92</t>
+  </si>
+  <si>
+    <t>TESTOR (TEST)</t>
+  </si>
+  <si>
+    <t>0xECD033C5D9AC7a6A8270e3D18B35692f8a9081C8</t>
+  </si>
+  <si>
+    <t>467 Wrapped Ether (WETH) + 2145 TESTOR (TEST)</t>
+  </si>
+  <si>
+    <t>0x494b0294148108F92580Ac1b501A4C9e6133fca9</t>
+  </si>
+  <si>
+    <t>EPEP (EPEP)</t>
+  </si>
+  <si>
+    <t>0x2A712464A3Eea099E101AEF3911Cc2339e815dfD</t>
+  </si>
+  <si>
+    <t>63245554 EPEP (EPEP) + 1 Wrapped Ether (WETH)</t>
+  </si>
+  <si>
+    <t>0x65fA4CEAB3B46cc098920CBd6B52545Dc7B4d614</t>
+  </si>
+  <si>
+    <t>Dodo (DODO)</t>
+  </si>
+  <si>
+    <t>0x1CD0A010A3233a3515e8E0639177D418Ff073b6e</t>
+  </si>
+  <si>
+    <t>2399999888999999158 Dodo (DODO) + 100000004638917 Wrapped Ether (WETH)</t>
+  </si>
+  <si>
+    <t>0xDa0DBef45FB703615eB3b73D07043242B891bb0B</t>
+  </si>
+  <si>
+    <t>INOWATTIO (INO)</t>
+  </si>
+  <si>
+    <t>0x3a313d31084046b61B31eEE59d75948015C00BD6</t>
+  </si>
+  <si>
+    <t>135290 INOWATTIO (INO) + 8 Wrapped Ether (WETH)</t>
+  </si>
+  <si>
+    <t>0xb676aA67860ECea407486022AD54f473057FD3FE</t>
+  </si>
+  <si>
+    <t>Hello World (hello)</t>
+  </si>
+  <si>
+    <t>0xb1eDe845808F5B78C3F932f2F3425861039D60B6</t>
+  </si>
+  <si>
+    <t>2026000000000000 Wrapped Ether (WETH) + 937844716764553042880004295 Hello World (hello)</t>
+  </si>
+  <si>
+    <t>0xC40D3967b7f7B706b08f5B54761c01E169CdAC8b</t>
+  </si>
+  <si>
+    <t>OP AI Nodes (OPAI)</t>
+  </si>
+  <si>
+    <t>0xD493017bcE81A79512E49C99A58c30FcbA02edbE</t>
+  </si>
+  <si>
+    <t>340 Wrapped Ether (WETH) + 59060826738617 OP AI Nodes (OPAI)</t>
+  </si>
+  <si>
+    <t>0x17E06Ff8672fF2BfA28EC8D150EA50741d080685</t>
+  </si>
+  <si>
+    <t>Husky Doge (HUSKY)</t>
+  </si>
+  <si>
+    <t>0x54a15EDc72Dac8Ec83396859892c6eb134a1eB34</t>
+  </si>
+  <si>
+    <t>1 Optimism (OP) + 14208941 Husky Doge (HUSKY)</t>
+  </si>
+  <si>
+    <t>0x3765Bd433556B29CC501eb1C9CFF228C1bf5158D</t>
+  </si>
+  <si>
+    <t>LERNITAS (2192)</t>
+  </si>
+  <si>
+    <t>0x3Ed9AcAac7Bd974eB83a8eA6432a239e3C829D5D</t>
+  </si>
+  <si>
+    <t>10480630780195653530861 LERNITAS (2192) + 15051635353892598 Wrapped Ether (WETH)</t>
+  </si>
+  <si>
+    <t>0xcbEbca932d46C82eB2bf173B2A65F9175e7580fd</t>
+  </si>
+  <si>
+    <t>DeepChain (DeepChain)</t>
+  </si>
+  <si>
+    <t>0x091D1012A7be2d503f3cf8762C87077767D8de0b</t>
+  </si>
+  <si>
+    <t>3357427896189640292525501 DeepChain (DeepChain) + 300030044999797 Wrapped Ether (WETH)</t>
+  </si>
+  <si>
+    <t>0x2EA784b4cDFaCeBEBb0B1271A58B2Dc62f44b238</t>
+  </si>
+  <si>
+    <t>Really not USD (RNUSD)</t>
+  </si>
+  <si>
+    <t>0x902A67bD38Dbce9A3cF28C2E86C1C5d3261a983b</t>
+  </si>
+  <si>
+    <t>999999003000994009 Really not USD (RNUSD) + 1000001 Tether USD (USDT)</t>
+  </si>
+  <si>
+    <t>0xFb77452FcE61d31bf2f6Ba6b22FAdAcA92300020</t>
+  </si>
+  <si>
+    <t>Whale (🐋)</t>
+  </si>
+  <si>
+    <t>0x2B8123B78638aBBfC85938833Cc9F5B575007155</t>
+  </si>
+  <si>
+    <t>37490726229774400127392586447505 Whale (🐋) + 3605132666050570 Wrapped Ether (WETH)</t>
+  </si>
+  <si>
+    <t>0x717EcDD3D0E2EAFfc4B4D0F3dD42C84F425ad18F</t>
+  </si>
+  <si>
+    <t>test token (TEST)</t>
+  </si>
+  <si>
+    <t>0xF8e724b645c402FDeC321892AdF86e458f00E500</t>
+  </si>
+  <si>
+    <t>1 Wrapped Ether (WETH) + 1870828694 test token (TEST)</t>
+  </si>
+  <si>
+    <t>0xD25561893d2015Ab47E679C5C3FEa3b06dd245D8</t>
+  </si>
+  <si>
+    <t>AIHub Coin (AIH)</t>
+  </si>
+  <si>
+    <t>0x2E6ca4bCC070C59F9370e3fF0EE6F2a92a959577</t>
+  </si>
+  <si>
+    <t>49900498406178080907 AIHub Coin (AIH) + 50100000 Tether USD (USDT)</t>
+  </si>
+  <si>
+    <t>0xa3B8d38dD99B3c9518211fB6FA065de73cca8Ec7</t>
+  </si>
+  <si>
+    <t>Meta Land Coin (MLC)</t>
+  </si>
+  <si>
+    <t>0x48Bffd5d53DA881DCADc1C1ea76326c15d019bFb</t>
+  </si>
+  <si>
+    <t>49900498406178080907 Meta Land Coin (MLC) + 50100000 Tether USD (USDT)</t>
+  </si>
+  <si>
+    <t>0x6A168F44cE9A6a43D9E6161B5237C177311C5ee0</t>
+  </si>
+  <si>
+    <t>0x740B666DC797f3122e3559ca8Ad87CD490AB6c01</t>
+  </si>
+  <si>
+    <t>100000000000000 Wrapped Ether (WETH) + 3000000000000 Dodo (DODO)</t>
+  </si>
+  <si>
+    <t>0xC36aB7527477744aB36F59aF89898055d0EEd4e3</t>
+  </si>
+  <si>
+    <t>550481883 Optimism (OP) + 1 Tether USD (USDT)</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,9 +816,838 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G36"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" t="s">
+        <v>100</v>
+      </c>
+      <c r="G25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" t="s">
+        <v>104</v>
+      </c>
+      <c r="G26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" t="s">
+        <v>108</v>
+      </c>
+      <c r="G27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" t="s">
+        <v>116</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>127</v>
+      </c>
+      <c r="F32" t="s">
+        <v>128</v>
+      </c>
+      <c r="G32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" t="s">
+        <v>136</v>
+      </c>
+      <c r="E34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" t="s">
+        <v>91</v>
+      </c>
+      <c r="F35" t="s">
+        <v>139</v>
+      </c>
+      <c r="G35" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>